<commit_message>
Modificaciones y adiciones horario
- Se agregó el horario de clases completo.
- Se cambió las franjas horarias por otras más detalladas.
- Se agregaron colores para identificar cada asignatura.
</commit_message>
<xml_diff>
--- a/Programación.xlsx
+++ b/Programación.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paola\OneDrive\Documentos\GitHub\Programacion-mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B17DAF6-CB60-44DE-8613-B71176A755D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F14367-9C66-4508-AB31-3C1F3CE34C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>LUNES</t>
   </si>
@@ -52,13 +52,79 @@
   </si>
   <si>
     <t>HORA</t>
+  </si>
+  <si>
+    <t>6:00 - 7:00 a. m.</t>
+  </si>
+  <si>
+    <t>7:00 - 8:00 a. m.</t>
+  </si>
+  <si>
+    <t>8:00 - 9:00 a. m.</t>
+  </si>
+  <si>
+    <t>9:00 - 10:00 a. m.</t>
+  </si>
+  <si>
+    <t>10:00 - 11:00 a. m.</t>
+  </si>
+  <si>
+    <t>11:00 - 12:00 m.</t>
+  </si>
+  <si>
+    <t>1: 00 12:00 p. m.</t>
+  </si>
+  <si>
+    <t>1:00 - 2:00 p. m.</t>
+  </si>
+  <si>
+    <t>2:00 - 3:00 p. m.</t>
+  </si>
+  <si>
+    <t>3:00 - 4:00 p. m.</t>
+  </si>
+  <si>
+    <t>4:00 - 5:00 p. m.</t>
+  </si>
+  <si>
+    <t>5:00 - 6:00 p. m.</t>
+  </si>
+  <si>
+    <t>6:00 - 7:00 p. m.</t>
+  </si>
+  <si>
+    <t>7:00 - 8:00 p. m.</t>
+  </si>
+  <si>
+    <t>Informática II</t>
+  </si>
+  <si>
+    <t>Álgebra y trigonometría</t>
+  </si>
+  <si>
+    <t>Cálculo diferencial</t>
+  </si>
+  <si>
+    <t>Inglés IV</t>
+  </si>
+  <si>
+    <t>Cálculo diferencia</t>
+  </si>
+  <si>
+    <t>Matemáticas discretas</t>
+  </si>
+  <si>
+    <t>Laboratorio - informática II</t>
+  </si>
+  <si>
+    <t>Álgebra y trigonometria</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,13 +148,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF05646"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3FC2E1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEA840"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD9239"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,21 +207,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -126,6 +251,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFD9239"/>
+      <color rgb="FFFD7F17"/>
+      <color rgb="FFEEA840"/>
+      <color rgb="FFEDC041"/>
+      <color rgb="FFEDB26E"/>
+      <color rgb="FF66FF66"/>
+      <color rgb="FF3FC2E1"/>
+      <color rgb="FFF05646"/>
+      <color rgb="FF20AED0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -400,137 +538,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
-    <col min="2" max="8" width="15.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="1" customWidth="1"/>
+    <col min="2" max="8" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>0.25</v>
+      <c r="A3" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>0.29166666666666669</v>
+      <c r="A4" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C5" s="1"/>
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>0.375</v>
-      </c>
-      <c r="C6" s="1"/>
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C7" s="1"/>
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>0.45833333333333331</v>
-      </c>
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>0.54166666666666663</v>
-      </c>
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>0.58333333333333337</v>
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>0.625</v>
-      </c>
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>0.66666666666666663</v>
-      </c>
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>0.70833333333333337</v>
-      </c>
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>0.75</v>
-      </c>
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>0.79166666666666663</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="A16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="12">
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F7:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Creación de tiempo de estudio
- Adición de horarios de tiempo de estudio de las asignaturas.
- Creación de espacio para trabajo en proyecto de semillero.
</commit_message>
<xml_diff>
--- a/Programación.xlsx
+++ b/Programación.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paola\OneDrive\Documentos\GitHub\Programacion-mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B17DAF6-CB60-44DE-8613-B71176A755D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64278825-CE57-469E-BD8E-255565DDF501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>LUNES</t>
   </si>
@@ -52,13 +52,94 @@
   </si>
   <si>
     <t>HORA</t>
+  </si>
+  <si>
+    <t>6:00 - 7:00 a. m.</t>
+  </si>
+  <si>
+    <t>7:00 - 8:00 a. m.</t>
+  </si>
+  <si>
+    <t>8:00 - 9:00 a. m.</t>
+  </si>
+  <si>
+    <t>9:00 - 10:00 a. m.</t>
+  </si>
+  <si>
+    <t>10:00 - 11:00 a. m.</t>
+  </si>
+  <si>
+    <t>11:00 - 12:00 m.</t>
+  </si>
+  <si>
+    <t>1: 00 12:00 p. m.</t>
+  </si>
+  <si>
+    <t>1:00 - 2:00 p. m.</t>
+  </si>
+  <si>
+    <t>2:00 - 3:00 p. m.</t>
+  </si>
+  <si>
+    <t>3:00 - 4:00 p. m.</t>
+  </si>
+  <si>
+    <t>4:00 - 5:00 p. m.</t>
+  </si>
+  <si>
+    <t>5:00 - 6:00 p. m.</t>
+  </si>
+  <si>
+    <t>6:00 - 7:00 p. m.</t>
+  </si>
+  <si>
+    <t>7:00 - 8:00 p. m.</t>
+  </si>
+  <si>
+    <t>Informática II</t>
+  </si>
+  <si>
+    <t>Álgebra y trigonometría</t>
+  </si>
+  <si>
+    <t>Cálculo diferencial</t>
+  </si>
+  <si>
+    <t>Inglés IV</t>
+  </si>
+  <si>
+    <t>Cálculo diferencia</t>
+  </si>
+  <si>
+    <t>Matemáticas discretas</t>
+  </si>
+  <si>
+    <t>Laboratorio - informática II</t>
+  </si>
+  <si>
+    <t>Álgebra y trigonometria</t>
+  </si>
+  <si>
+    <t>Sesión de estudio 1: álgebra</t>
+  </si>
+  <si>
+    <t>Sesión de estudio 2: cálculo</t>
+  </si>
+  <si>
+    <t>Sesión de estudio 3: informática</t>
+  </si>
+  <si>
+    <t>Sesión de estudio: matemáticas</t>
+  </si>
+  <si>
+    <t>Trabajo en proyecto de semillero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,13 +163,65 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF05646"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3FC2E1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEA840"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD9239"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,22 +236,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -126,6 +280,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFD9239"/>
+      <color rgb="FFFD7F17"/>
+      <color rgb="FFEEA840"/>
+      <color rgb="FFEDC041"/>
+      <color rgb="FFEDB26E"/>
+      <color rgb="FF66FF66"/>
+      <color rgb="FF3FC2E1"/>
+      <color rgb="FFF05646"/>
+      <color rgb="FF20AED0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -400,137 +567,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
-    <col min="2" max="8" width="15.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="1" customWidth="1"/>
+    <col min="2" max="8" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>0.25</v>
+      <c r="A3" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>0.29166666666666669</v>
+      <c r="A4" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C5" s="1"/>
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>0.375</v>
-      </c>
-      <c r="C6" s="1"/>
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C7" s="1"/>
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>0.45833333333333331</v>
-      </c>
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>0.5</v>
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="H9" s="12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>0.54166666666666663</v>
-      </c>
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="4"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>0.58333333333333337</v>
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>0.625</v>
-      </c>
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="6"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>0.66666666666666663</v>
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="H13" s="12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>0.70833333333333337</v>
-      </c>
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="4"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>0.75</v>
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="H15" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>0.79166666666666663</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="A16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="4"/>
+      <c r="H16" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="25">
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D15:D16"/>
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>